<commit_message>
CSV 데이터를 Scriptable Object로 자동 변환
</commit_message>
<xml_diff>
--- a/Assets/100_Data/XlsxFiles/Engine_Data.xlsx
+++ b/Assets/100_Data/XlsxFiles/Engine_Data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="59">
   <si>
     <t>ID</t>
   </si>
@@ -140,6 +140,82 @@
   <si>
     <t xml:space="preserve">엔진 위치의 상부 시설을 작동시킵니다. </t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GreenEngine_1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GreenEngine_2</t>
+  </si>
+  <si>
+    <t>GreenEngine_3</t>
+  </si>
+  <si>
+    <t>GreenEngine_4</t>
+  </si>
+  <si>
+    <t>RedEngine_1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RedEngine_2</t>
+  </si>
+  <si>
+    <t>RedEngine_3</t>
+  </si>
+  <si>
+    <t>RedEngine_4</t>
+  </si>
+  <si>
+    <t>BlueEngine_1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BlueEngine_2</t>
+  </si>
+  <si>
+    <t>BlueEngine_3</t>
+  </si>
+  <si>
+    <t>BlueEngine_4</t>
+  </si>
+  <si>
+    <t>PurpleEngine_1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>PurpleEngine_2</t>
+  </si>
+  <si>
+    <t>PurpleEngine_3</t>
+  </si>
+  <si>
+    <t>PurpleEngine_4</t>
+  </si>
+  <si>
+    <t>YellowEngine_1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>YellowEngine_2</t>
+  </si>
+  <si>
+    <t>YellowEngine_3</t>
+  </si>
+  <si>
+    <t>YellowEngine_4</t>
+  </si>
+  <si>
+    <t>SpecialEngine_1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SpecialEngine_2</t>
   </si>
 </sst>
 </file>
@@ -882,10 +958,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="표1" displayName="표1" ref="A1:G23" totalsRowShown="0">
-  <autoFilter ref="A1:G23"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="표1" displayName="표1" ref="A1:H23" totalsRowShown="0">
+  <autoFilter ref="A1:H23"/>
+  <tableColumns count="8">
     <tableColumn id="1" name="ID"/>
+    <tableColumn id="8" name="Name"/>
     <tableColumn id="6" name="EngineId"/>
     <tableColumn id="5" name="DisplayName"/>
     <tableColumn id="2" name="Type"/>
@@ -1160,536 +1237,606 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.375" customWidth="1"/>
+    <col min="2" max="2" width="22.75" customWidth="1"/>
     <col min="3" max="3" width="18.375" customWidth="1"/>
     <col min="4" max="4" width="13.375" customWidth="1"/>
     <col min="7" max="7" width="35.875" customWidth="1"/>
+    <col min="8" max="8" width="34.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>201001</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2">
         <v>201</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2">
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>201002</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3">
         <v>201</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3">
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>201003</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4">
         <v>201</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4">
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>201004</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5">
         <v>201</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
         <v>8</v>
       </c>
-      <c r="G5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>202001</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6">
         <v>202</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6">
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6">
         <v>1</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>5</v>
       </c>
-      <c r="G6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>202002</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7">
         <v>202</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>19</v>
       </c>
-      <c r="D7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7">
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7">
         <v>2</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>6</v>
       </c>
-      <c r="G7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>202003</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8">
         <v>202</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>20</v>
       </c>
-      <c r="D8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8">
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8">
         <v>3</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>7</v>
       </c>
-      <c r="G8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>202004</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9">
         <v>202</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>21</v>
       </c>
-      <c r="D9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9">
-        <v>4</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9" t="s">
         <v>8</v>
       </c>
-      <c r="G9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>203001</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10">
         <v>203</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>22</v>
       </c>
-      <c r="D10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10">
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10">
         <v>1</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>5</v>
       </c>
-      <c r="G10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>203002</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11">
         <v>203</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>23</v>
       </c>
-      <c r="D11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11">
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11">
         <v>2</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>6</v>
       </c>
-      <c r="G11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>203003</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12">
         <v>203</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>24</v>
       </c>
-      <c r="D12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12">
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12">
         <v>3</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>7</v>
       </c>
-      <c r="G12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>203004</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13">
         <v>203</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>25</v>
       </c>
-      <c r="D13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13">
-        <v>4</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="G13" t="s">
         <v>8</v>
       </c>
-      <c r="G13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>204001</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14">
         <v>204</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>26</v>
       </c>
-      <c r="D14" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14">
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14">
         <v>1</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>5</v>
       </c>
-      <c r="G14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>204002</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15">
         <v>204</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>27</v>
       </c>
-      <c r="D15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15">
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15">
         <v>2</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>6</v>
       </c>
-      <c r="G15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>204003</v>
       </c>
-      <c r="B16">
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16">
         <v>204</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>28</v>
       </c>
-      <c r="D16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16">
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16">
         <v>3</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>7</v>
       </c>
-      <c r="G16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>204004</v>
       </c>
-      <c r="B17">
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17">
         <v>204</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>29</v>
       </c>
-      <c r="D17" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17">
-        <v>4</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>4</v>
+      </c>
+      <c r="G17" t="s">
         <v>8</v>
       </c>
-      <c r="G17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>205001</v>
       </c>
-      <c r="B18">
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18">
         <v>205</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>30</v>
       </c>
-      <c r="D18" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18">
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18">
         <v>1</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>5</v>
       </c>
-      <c r="G18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>205002</v>
       </c>
-      <c r="B19">
+      <c r="B19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19">
         <v>205</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>31</v>
       </c>
-      <c r="D19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19">
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19">
         <v>2</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>6</v>
       </c>
-      <c r="G19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>205003</v>
       </c>
-      <c r="B20">
+      <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20">
         <v>205</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>32</v>
       </c>
-      <c r="D20" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20">
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20">
         <v>3</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>7</v>
       </c>
-      <c r="G20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>205004</v>
       </c>
-      <c r="B21">
+      <c r="B21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21">
         <v>205</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>33</v>
       </c>
-      <c r="D21" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21">
-        <v>4</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21">
+        <v>4</v>
+      </c>
+      <c r="G21" t="s">
         <v>8</v>
       </c>
-      <c r="G21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>211001</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="C22" s="2"/>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="2"/>
+      <c r="E22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="2">
+      <c r="F22" s="2">
         <v>1</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="G22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G22" s="7"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>211002</v>
       </c>
-      <c r="B23" s="6"/>
+      <c r="B23" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="C23" s="6"/>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="6"/>
+      <c r="E23" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="6">
+      <c r="F23" s="6">
         <v>2</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="G23" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>